<commit_message>
Test file update and light refactoring
</commit_message>
<xml_diff>
--- a/src/test/resources/input.xlsx
+++ b/src/test/resources/input.xlsx
@@ -154,6 +154,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -175,6 +176,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -252,16 +254,15 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.9897959183674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Refactoring import task implementation to detect and ignore empty rows
</commit_message>
<xml_diff>
--- a/src/test/resources/input.xlsx
+++ b/src/test/resources/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">es</t>
   </si>
   <si>
-    <t xml:space="preserve">trad.key.key_1</t>
+    <t xml:space="preserve">trad_key_key.1</t>
   </si>
   <si>
     <t xml:space="preserve">Texte de l'application écrit en français n°1</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Texto de la aplicación escrito en español n°1</t>
   </si>
   <si>
-    <t xml:space="preserve">trad.key.key_2</t>
+    <t xml:space="preserve">trad_key_key.2</t>
   </si>
   <si>
     <t xml:space="preserve">Texte de l'application écrit en français n°2</t>
@@ -58,7 +58,16 @@
     <t xml:space="preserve">Texto de la aplicación escrito en español n°2</t>
   </si>
   <si>
-    <t xml:space="preserve">trad.key.key_3</t>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">trad_key_key.3</t>
   </si>
   <si>
     <t xml:space="preserve">Texte de l'application avec un paramètre #</t>
@@ -70,7 +79,7 @@
     <t xml:space="preserve">Texto de la aplicación con un parámetro #</t>
   </si>
   <si>
-    <t xml:space="preserve">trad.key.key_4</t>
+    <t xml:space="preserve">trad_key_key.4</t>
   </si>
   <si>
     <t xml:space="preserve">Texte de l'application avec deux paramètres # et #</t>
@@ -82,7 +91,7 @@
     <t xml:space="preserve">Texto de la aplicación con dos parámetros # y #</t>
   </si>
   <si>
-    <t xml:space="preserve">trad.key.key_5</t>
+    <t xml:space="preserve">  trad_key_key.5  </t>
   </si>
   <si>
     <t xml:space="preserve">Texte avec "guillemets" internes</t>
@@ -94,7 +103,7 @@
     <t xml:space="preserve">Texto con "citas" internas</t>
   </si>
   <si>
-    <t xml:space="preserve">trad.key.key_6</t>
+    <t xml:space="preserve">trad_key_key.6</t>
   </si>
   <si>
     <t xml:space="preserve">Texte avec nombre %1$d</t>
@@ -106,7 +115,7 @@
     <t xml:space="preserve">Texto con número %1$d</t>
   </si>
   <si>
-    <t xml:space="preserve">trad.key.key_7:one</t>
+    <t xml:space="preserve">trad_key_key.7:one</t>
   </si>
   <si>
     <t xml:space="preserve">Une pomme</t>
@@ -118,7 +127,7 @@
     <t xml:space="preserve">Una manzana</t>
   </si>
   <si>
-    <t xml:space="preserve">trad.key.key_7:two</t>
+    <t xml:space="preserve">trad_key_key.7:two</t>
   </si>
   <si>
     <t xml:space="preserve">Deux pommes</t>
@@ -130,7 +139,7 @@
     <t xml:space="preserve">Dos manzanas</t>
   </si>
   <si>
-    <t xml:space="preserve">trad.key.key_7:many</t>
+    <t xml:space="preserve">trad_key_key.7:many</t>
   </si>
   <si>
     <t xml:space="preserve">Plein de pommes</t>
@@ -140,16 +149,23 @@
   </si>
   <si>
     <t xml:space="preserve">Muchas manzanas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trad_key_key.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only in english</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -178,13 +194,24 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF336699"/>
+        <bgColor rgb="FF0066CC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,17 +248,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -243,6 +290,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF336699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -251,161 +358,206 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="43.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="2" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>